<commit_message>
Getting closer on matrix printing
</commit_message>
<xml_diff>
--- a/data/Example.xlsx
+++ b/data/Example.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE110AA-C06F-1245-ADFB-951C99FB0B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44BCDD6-982C-0A49-B10B-8CDC601F3FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="example1">Sheet1!$B$6</definedName>
     <definedName name="example2">Sheet2!$D$7</definedName>
+    <definedName name="Rmat">Sheet3!$E$12:$H$15</definedName>
   </definedNames>
   <calcPr calcId="140000"/>
   <extLst>
@@ -27,6 +29,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Resources [of Product 1]</t>
+  </si>
+  <si>
+    <t>Resources [of Product 2]</t>
+  </si>
+  <si>
+    <t>Resources [of Product 3]</t>
+  </si>
+  <si>
+    <t>Product 1</t>
+  </si>
+  <si>
+    <t>Product 2</t>
+  </si>
+  <si>
+    <t>Product 3</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -60,8 +91,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036F81E4-74E8-764C-B993-0879D3DB740A}">
   <dimension ref="D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -442,4 +482,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545274DC-34DC-FF41-A18E-A55E6B091650}">
+  <dimension ref="E12:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="8" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="5:8" ht="53" x14ac:dyDescent="0.2">
+      <c r="F12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>42</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <v>43</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Getting closer to matrix printout.
</commit_message>
<xml_diff>
--- a/data/Example.xlsx
+++ b/data/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44BCDD6-982C-0A49-B10B-8CDC601F3FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB6F9B9-E111-DD4A-9A52-8F3430A5ABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
     <t>Product 2</t>
   </si>
   <si>
-    <t>Product 3</t>
+    <t>P3</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="E12:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:H15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Working on statepoint table.
</commit_message>
<xml_diff>
--- a/data/Example.xlsx
+++ b/data/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB6F9B9-E111-DD4A-9A52-8F3430A5ABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E93FDA-0B26-3148-8CFF-067AC3DA4B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,21 @@
     <definedName name="example1">Sheet1!$B$6</definedName>
     <definedName name="example2">Sheet2!$D$7</definedName>
     <definedName name="Rmat">Sheet3!$E$12:$H$15</definedName>
+    <definedName name="statepoint_table">Sheet3!$F$29:$O$33</definedName>
   </definedNames>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Resources [of Product 1]</t>
   </si>
@@ -50,6 +62,99 @@
   </si>
   <si>
     <t>P3</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>[kgm]</t>
+  </si>
+  <si>
+    <t>[kJm]</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>ln(yi)</t>
+  </si>
+  <si>
+    <t>[kgi]</t>
+  </si>
+  <si>
+    <t>[kgi/moli]</t>
+  </si>
+  <si>
+    <t>[moli]</t>
+  </si>
+  <si>
+    <t>[kJi/moli]</t>
+  </si>
+  <si>
+    <t>[moli/molm]</t>
+  </si>
+  <si>
+    <t>[-]</t>
+  </si>
+  <si>
+    <t>[kJi/molm]</t>
+  </si>
+  <si>
+    <t>[kJi]</t>
+  </si>
+  <si>
+    <t>Blast furnace mixture</t>
+  </si>
+  <si>
+    <t>Fe2O3</t>
+  </si>
+  <si>
+    <t>SiO2</t>
+  </si>
+  <si>
+    <t>CaO</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>[kgm/molm]</t>
+  </si>
+  <si>
+    <t>[molm]</t>
+  </si>
+  <si>
+    <t>[kJm/molm]</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>bch,i</t>
+  </si>
+  <si>
+    <t>yi</t>
+  </si>
+  <si>
+    <t>Bm</t>
+  </si>
+  <si>
+    <t>bi</t>
+  </si>
+  <si>
+    <t>bm</t>
+  </si>
+  <si>
+    <t>bc,i</t>
   </si>
 </sst>
 </file>
@@ -486,10 +591,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545274DC-34DC-FF41-A18E-A55E6B091650}">
-  <dimension ref="E12:H15"/>
+  <dimension ref="D12:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +643,276 @@
         <v>44</v>
       </c>
     </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>8</v>
+      </c>
+      <c r="O24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="N25">
+        <v>1309.8157778632656</v>
+      </c>
+      <c r="O25">
+        <v>7072531.8830895294</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" t="s">
+        <v>36</v>
+      </c>
+      <c r="M27" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" t="s">
+        <v>15</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" t="s">
+        <v>18</v>
+      </c>
+      <c r="O28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29">
+        <v>881.06000000000006</v>
+      </c>
+      <c r="G29">
+        <v>0.1596882</v>
+      </c>
+      <c r="H29">
+        <v>5517.3769884061567</v>
+      </c>
+      <c r="I29">
+        <v>17.358400000000074</v>
+      </c>
+      <c r="J29">
+        <v>0.21197353787675174</v>
+      </c>
+      <c r="K29">
+        <v>-1.5512938334370325</v>
+      </c>
+      <c r="L29">
+        <v>-3.5229403607560474</v>
+      </c>
+      <c r="M29">
+        <v>13.835459639244027</v>
+      </c>
+      <c r="N29">
+        <v>2.9327513278815638</v>
+      </c>
+      <c r="O29">
+        <v>76335.446637587142</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>118.94000000000001</v>
+      </c>
+      <c r="G30">
+        <v>6.00843E-2</v>
+      </c>
+      <c r="H30">
+        <v>1979.5520626852608</v>
+      </c>
+      <c r="I30">
+        <v>1.5260000000000673</v>
+      </c>
+      <c r="J30">
+        <v>7.6052924246496442E-2</v>
+      </c>
+      <c r="K30">
+        <v>-2.5763258093856205</v>
+      </c>
+      <c r="L30">
+        <v>-5.8507563046472342</v>
+      </c>
+      <c r="M30">
+        <v>-4.3247563046471669</v>
+      </c>
+      <c r="N30">
+        <v>-0.32891036362188886</v>
+      </c>
+      <c r="O30">
+        <v>-8561.0802634753836</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31">
+        <v>111.00813284002646</v>
+      </c>
+      <c r="G31">
+        <v>5.6077400000000006E-2</v>
+      </c>
+      <c r="H31">
+        <v>1979.5520626852608</v>
+      </c>
+      <c r="I31">
+        <v>122.25799999999992</v>
+      </c>
+      <c r="J31">
+        <v>7.6052924246496442E-2</v>
+      </c>
+      <c r="K31">
+        <v>-2.5763258093856205</v>
+      </c>
+      <c r="L31">
+        <v>-5.8507563046472342</v>
+      </c>
+      <c r="M31">
+        <v>116.40724369535269</v>
+      </c>
+      <c r="N31">
+        <v>8.8531112865061079</v>
+      </c>
+      <c r="O31">
+        <v>230434.19936864119</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32">
+        <v>198.80764502323905</v>
+      </c>
+      <c r="G32">
+        <v>1.2010999999999999E-2</v>
+      </c>
+      <c r="H32">
+        <v>16552.130965218472</v>
+      </c>
+      <c r="I32">
+        <v>410.3</v>
+      </c>
+      <c r="J32">
+        <v>0.63592061363025532</v>
+      </c>
+      <c r="K32">
+        <v>-0.45268154476892275</v>
+      </c>
+      <c r="L32">
+        <v>-1.0280258003104901</v>
+      </c>
+      <c r="M32">
+        <v>409.27197419968951</v>
+      </c>
+      <c r="N32">
+        <v>260.26448497473257</v>
+      </c>
+      <c r="O32">
+        <v>6774323.3173467768</v>
+      </c>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>1309.8157778632656</v>
+      </c>
+      <c r="G33">
+        <v>0.28786090000000003</v>
+      </c>
+      <c r="H33">
+        <v>26028.612078995153</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>7072531.8830895294</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N34" t="s">
+        <v>28</v>
+      </c>
+      <c r="O34" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mass and Energy tables format
</commit_message>
<xml_diff>
--- a/data/Example.xlsx
+++ b/data/Example.xlsx
@@ -5,22 +5,42 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinschuman/Documents/github/MaterialExergyPaper/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E93FDA-0B26-3148-8CFF-067AC3DA4B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA87FB23-D462-5F4F-BAC1-6B1B40989925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="4880" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Energy and Mass Formatting" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="b_ch_Al2O3">[1]Constants!$E$24</definedName>
+    <definedName name="b_ch_C12H23">[1]Constants!$E$41</definedName>
+    <definedName name="b_ch_Fe2O3">[1]Constants!$E$10</definedName>
+    <definedName name="b_ch_K2O">[1]Constants!$E$27</definedName>
+    <definedName name="b_ch_P">[1]Constants!$E$28</definedName>
+    <definedName name="b_ch_S">[1]Constants!$E$22</definedName>
+    <definedName name="b_ch_SiO2">[1]Constants!$E$14</definedName>
     <definedName name="example1">Sheet1!$B$6</definedName>
     <definedName name="example2">Sheet2!$D$7</definedName>
+    <definedName name="LHV_Diesel">[1]Constants!$W$13</definedName>
+    <definedName name="MW_Al2O3">[1]Constants!$D$24</definedName>
+    <definedName name="MW_C12H23">[1]Constants!$D$41</definedName>
+    <definedName name="MW_Fe2O3">[1]Constants!$D$10</definedName>
+    <definedName name="MW_K2O">[1]Constants!$D$27</definedName>
+    <definedName name="MW_P">[1]Constants!$D$28</definedName>
+    <definedName name="MW_S">[1]Constants!$D$22</definedName>
+    <definedName name="MW_SIO2">[1]Constants!$D$14</definedName>
     <definedName name="Rmat">Sheet3!$E$12:$H$15</definedName>
+    <definedName name="RT0">[1]Constants!$M$5</definedName>
     <definedName name="statepoint_table">Sheet3!$F$29:$O$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>Resources [of Product 1]</t>
   </si>
@@ -155,19 +175,92 @@
   </si>
   <si>
     <t>bc,i</t>
+  </si>
+  <si>
+    <t>xi</t>
+  </si>
+  <si>
+    <t>MWi</t>
+  </si>
+  <si>
+    <t>bc,i = R T0 ln(yi)</t>
+  </si>
+  <si>
+    <t>bi = bch,i + bc,i</t>
+  </si>
+  <si>
+    <t>bm = yi bi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [kgi/kgm]</t>
+  </si>
+  <si>
+    <t>K2O</t>
+  </si>
+  <si>
+    <t>Al2O3</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>[i]</t>
+  </si>
+  <si>
+    <t>C12H23</t>
+  </si>
+  <si>
+    <t>[kJ]</t>
+  </si>
+  <si>
+    <t>Energy Sources</t>
+  </si>
+  <si>
+    <t>Mass Sources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -184,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -192,11 +285,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -206,6 +376,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -222,6 +431,109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Constants"/>
+      <sheetName val="BF Calculator"/>
+      <sheetName val="Ore-&gt;PI"/>
+      <sheetName val="Mass RUVY matrices (mat level)"/>
+      <sheetName val="B RUVY matrices (mat level)"/>
+      <sheetName val="Energy RUVY matrices"/>
+      <sheetName val="Energy X"/>
+      <sheetName val="Efficiencies"/>
+      <sheetName val="Waste"/>
+      <sheetName val="Methane Combustion - EES"/>
+      <sheetName val="Tables for Paper"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="M5">
+            <v>2.2709690999999999</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="D10">
+            <v>0.1596882</v>
+          </cell>
+          <cell r="E10">
+            <v>17.358400000000074</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="W13">
+            <v>43000</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="D14">
+            <v>6.00843E-2</v>
+          </cell>
+          <cell r="E14">
+            <v>1.5260000000000673</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="D22">
+            <v>3.2066000000000004E-2</v>
+          </cell>
+          <cell r="E22">
+            <v>607.29999999999995</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="D24">
+            <v>0.10196127799999999</v>
+          </cell>
+          <cell r="E24">
+            <v>31.875999999999976</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="D27">
+            <v>9.4196000000000002E-2</v>
+          </cell>
+          <cell r="E27">
+            <v>412.83199999999999</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="D28">
+            <v>3.0973762000000002E-2</v>
+          </cell>
+          <cell r="E28">
+            <v>873.60807999999997</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="D41">
+            <v>0.16731462</v>
+          </cell>
+          <cell r="E41">
+            <v>7141.5943565339712</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545274DC-34DC-FF41-A18E-A55E6B091650}">
   <dimension ref="D12:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F29" sqref="F29:O33"/>
     </sheetView>
   </sheetViews>
@@ -915,4 +1227,667 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7457CBA-7643-2342-AA62-D18E6247C290}">
+  <dimension ref="A11:N32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="4"/>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="7">
+        <v>881.06000000000006</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.87081274068002201</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.1596882</v>
+      </c>
+      <c r="G13" s="7">
+        <v>5517.3769884061567</v>
+      </c>
+      <c r="H13" s="7">
+        <v>17.358400000000074</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.72360528709446914</v>
+      </c>
+      <c r="J13" s="7">
+        <v>-0.3235092188341952</v>
+      </c>
+      <c r="K13" s="7">
+        <v>-0.73467943953759529</v>
+      </c>
+      <c r="L13" s="7">
+        <v>16.62372056046248</v>
+      </c>
+      <c r="M13" s="7">
+        <v>12.029012088731683</v>
+      </c>
+      <c r="N13" s="7">
+        <v>91719.333281989995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4">
+        <v>118.94000000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.11755665604667312</v>
+      </c>
+      <c r="F14" s="4">
+        <v>6.00843E-2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1979.5520626852608</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1.5260000000000673</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.25961871767105915</v>
+      </c>
+      <c r="J14" s="4">
+        <v>-1.3485411947827832</v>
+      </c>
+      <c r="K14" s="4">
+        <v>-3.0624953834287818</v>
+      </c>
+      <c r="L14" s="4">
+        <v>-1.5364953834287145</v>
+      </c>
+      <c r="M14" s="4">
+        <v>-0.39890296115326523</v>
+      </c>
+      <c r="N14" s="4">
+        <v>-3041.5726055726927</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.249958452402667</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.2354206815346574E-3</v>
+      </c>
+      <c r="F15" s="4">
+        <v>9.4196000000000002E-2</v>
+      </c>
+      <c r="G15" s="4">
+        <v>13.269761480345949</v>
+      </c>
+      <c r="H15" s="4">
+        <v>412.83199999999999</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.7403323328889792E-3</v>
+      </c>
+      <c r="J15" s="4">
+        <v>-6.35367918807989</v>
+      </c>
+      <c r="K15" s="4">
+        <v>-14.429009107442518</v>
+      </c>
+      <c r="L15" s="4">
+        <v>398.40299089255745</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.69335360656999123</v>
+      </c>
+      <c r="N15" s="4">
+        <v>5286.7126622006763</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="4">
+        <v>9.9996676192213361</v>
+      </c>
+      <c r="E16" s="4">
+        <v>9.8833654522772589E-3</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.10196127799999999</v>
+      </c>
+      <c r="G16" s="4">
+        <v>98.073188325683176</v>
+      </c>
+      <c r="H16" s="4">
+        <v>31.875999999999976</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1.2862321669119157E-2</v>
+      </c>
+      <c r="J16" s="4">
+        <v>-4.3534530423208677</v>
+      </c>
+      <c r="K16" s="4">
+        <v>-9.8865573374116824</v>
+      </c>
+      <c r="L16" s="4">
+        <v>21.989442662588296</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.28283528485086268</v>
+      </c>
+      <c r="N16" s="4">
+        <v>2156.5747514248337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.38391581038081912</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3.7945063789993045E-4</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3.0973762000000002E-2</v>
+      </c>
+      <c r="G17" s="4">
+        <v>12.394871839617645</v>
+      </c>
+      <c r="H17" s="4">
+        <v>873.60807999999997</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1.6255903511491995E-3</v>
+      </c>
+      <c r="J17" s="4">
+        <v>-6.4218842361604729</v>
+      </c>
+      <c r="K17" s="4">
+        <v>-14.583900664097536</v>
+      </c>
+      <c r="L17" s="4">
+        <v>859.02417933590243</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1.3964214173323026</v>
+      </c>
+      <c r="N17" s="4">
+        <v>10647.494610001237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.13392411990028574</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.3236650159299899E-4</v>
+      </c>
+      <c r="F18" s="4">
+        <v>3.2066000000000004E-2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>4.1765146853454036</v>
+      </c>
+      <c r="H18" s="4">
+        <v>607.29999999999995</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5.4775088131446613E-4</v>
+      </c>
+      <c r="J18" s="4">
+        <v>-7.5096899705178952</v>
+      </c>
+      <c r="K18" s="4">
+        <v>-17.054273873626048</v>
+      </c>
+      <c r="L18" s="4">
+        <v>590.24572612637394</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.32330761667781832</v>
+      </c>
+      <c r="N18" s="4">
+        <v>2465.1699431291622</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1011.7674660019052</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.47896953999999997</v>
+      </c>
+      <c r="G19" s="7">
+        <v>7624.8433874224093</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7">
+        <v>14.326027053009392</v>
+      </c>
+      <c r="N19" s="7">
+        <v>109233.7126431732</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C20" s="4"/>
+      <c r="D20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="13">
+        <v>2.05024783499473</v>
+      </c>
+      <c r="N26" s="14">
+        <v>87512.008023532893</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C28" s="4"/>
+      <c r="D28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="15">
+        <v>88160.656904773379</v>
+      </c>
+      <c r="E30" s="15">
+        <v>2.05024783499473</v>
+      </c>
+      <c r="F30" s="15">
+        <v>0.16731462</v>
+      </c>
+      <c r="G30" s="15">
+        <v>12.253847482035521</v>
+      </c>
+      <c r="H30" s="15">
+        <v>7141.5943565339712</v>
+      </c>
+      <c r="I30" s="15">
+        <v>1</v>
+      </c>
+      <c r="J30" s="15">
+        <v>0</v>
+      </c>
+      <c r="K30" s="15">
+        <v>0</v>
+      </c>
+      <c r="L30" s="15">
+        <v>7141.5943565339712</v>
+      </c>
+      <c r="M30" s="15">
+        <v>7141.5943565339712</v>
+      </c>
+      <c r="N30" s="15">
+        <v>87512.008023532893</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="15">
+        <v>88160.656904773379</v>
+      </c>
+      <c r="E31" s="15">
+        <v>2.05024783499473</v>
+      </c>
+      <c r="F31" s="15">
+        <v>0.16731462</v>
+      </c>
+      <c r="G31" s="15">
+        <v>12.253847482035521</v>
+      </c>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15">
+        <v>7141.5943565339712</v>
+      </c>
+      <c r="N31" s="15">
+        <v>87512.008023532893</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A29:B31"/>
+    <mergeCell ref="A14:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commented table to read efficiencies
</commit_message>
<xml_diff>
--- a/data/Example.xlsx
+++ b/data/Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinschuman/Documents/github/MaterialExergyPaper/MaterialExergyPaper2025/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA87FB23-D462-5F4F-BAC1-6B1B40989925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA7CA22-71F7-604A-BE6E-411085A0B059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="4880" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="4880" windowWidth="25600" windowHeight="16160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,28 +20,36 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="b_ch_Al2O3">[1]Constants!$E$24</definedName>
     <definedName name="b_ch_C12H23">[1]Constants!$E$41</definedName>
+    <definedName name="b_ch_CaCO3">[2]Constants!$E$6</definedName>
     <definedName name="b_ch_Fe2O3">[1]Constants!$E$10</definedName>
     <definedName name="b_ch_K2O">[1]Constants!$E$27</definedName>
+    <definedName name="b_ch_MgCO3">[2]Constants!$E$29</definedName>
     <definedName name="b_ch_P">[1]Constants!$E$28</definedName>
     <definedName name="b_ch_S">[1]Constants!$E$22</definedName>
     <definedName name="b_ch_SiO2">[1]Constants!$E$14</definedName>
     <definedName name="example1">Sheet1!$B$6</definedName>
     <definedName name="example2">Sheet2!$D$7</definedName>
+    <definedName name="h_CaCO3">[2]Constants!$G$6</definedName>
+    <definedName name="h_MgCO3">[2]Constants!$G$29</definedName>
     <definedName name="LHV_Diesel">[1]Constants!$W$13</definedName>
+    <definedName name="Limestone_for_BF">[2]Calculators!$L$27</definedName>
     <definedName name="MW_Al2O3">[1]Constants!$D$24</definedName>
     <definedName name="MW_C12H23">[1]Constants!$D$41</definedName>
+    <definedName name="MW_CaCO3">[2]Constants!$D$6</definedName>
     <definedName name="MW_Fe2O3">[1]Constants!$D$10</definedName>
     <definedName name="MW_K2O">[1]Constants!$D$27</definedName>
+    <definedName name="MW_MgCO3">[2]Constants!$D$29</definedName>
     <definedName name="MW_P">[1]Constants!$D$28</definedName>
     <definedName name="MW_S">[1]Constants!$D$22</definedName>
     <definedName name="MW_SIO2">[1]Constants!$D$14</definedName>
     <definedName name="Rmat">Sheet3!$E$12:$H$15</definedName>
     <definedName name="RT0">[1]Constants!$M$5</definedName>
-    <definedName name="statepoint_table">Sheet3!$F$29:$O$33</definedName>
+    <definedName name="statepoint_table">Sheet3!$F$28:$Q$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>Resources [of Product 1]</t>
   </si>
@@ -96,9 +104,6 @@
     <t>[kJm]</t>
   </si>
   <si>
-    <t>MW</t>
-  </si>
-  <si>
     <t>ln(yi)</t>
   </si>
   <si>
@@ -126,21 +131,12 @@
     <t>[kJi]</t>
   </si>
   <si>
-    <t>Blast furnace mixture</t>
-  </si>
-  <si>
     <t>Fe2O3</t>
   </si>
   <si>
     <t>SiO2</t>
   </si>
   <si>
-    <t>CaO</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
@@ -168,15 +164,6 @@
     <t>Bm</t>
   </si>
   <si>
-    <t>bi</t>
-  </si>
-  <si>
-    <t>bm</t>
-  </si>
-  <si>
-    <t>bc,i</t>
-  </si>
-  <si>
     <t>xi</t>
   </si>
   <si>
@@ -223,6 +210,27 @@
   </si>
   <si>
     <t>Mass Sources</t>
+  </si>
+  <si>
+    <t>Limestone [from Beneficiation]</t>
+  </si>
+  <si>
+    <t>Limestone [from Limestone beneficiation]</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>[kJi/kgi]</t>
+  </si>
+  <si>
+    <t>CaCO3</t>
+  </si>
+  <si>
+    <t>MgCO3</t>
+  </si>
+  <si>
+    <t>[kJm/kgm]</t>
   </si>
 </sst>
 </file>
@@ -440,7 +448,10 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
+      <sheetName val="Draft 3 BF"/>
+      <sheetName val="BF"/>
       <sheetName val="Constants"/>
+      <sheetName val="Methane Combustion - EES"/>
       <sheetName val="BF Calculator"/>
       <sheetName val="Ore-&gt;PI"/>
       <sheetName val="Mass RUVY matrices (mat level)"/>
@@ -448,12 +459,11 @@
       <sheetName val="Energy RUVY matrices"/>
       <sheetName val="Energy X"/>
       <sheetName val="Efficiencies"/>
-      <sheetName val="Waste"/>
-      <sheetName val="Methane Combustion - EES"/>
-      <sheetName val="Tables for Paper"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
         <row r="5">
           <cell r="M5">
             <v>2.2709690999999999</v>
@@ -461,67 +471,87 @@
         </row>
         <row r="10">
           <cell r="D10">
-            <v>0.1596882</v>
+            <v>0.159692</v>
           </cell>
           <cell r="E10">
             <v>17.358400000000074</v>
           </cell>
         </row>
-        <row r="13">
-          <cell r="W13">
-            <v>43000</v>
-          </cell>
-        </row>
         <row r="14">
           <cell r="D14">
-            <v>6.00843E-2</v>
+            <v>6.0080000000000001E-2</v>
           </cell>
           <cell r="E14">
             <v>1.5260000000000673</v>
           </cell>
         </row>
-        <row r="22">
-          <cell r="D22">
-            <v>3.2066000000000004E-2</v>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Constants"/>
+      <sheetName val="Calculators"/>
+      <sheetName val="Fuel Exergy"/>
+      <sheetName val="Ore-&gt;PI"/>
+      <sheetName val="Energy X"/>
+      <sheetName val="MCC_B_RUVY_matrices_mat_level"/>
+      <sheetName val="MCC_M_RUVY_matrices_mat_level"/>
+      <sheetName val="MCC_h_RUVY_matrices_mat_level"/>
+      <sheetName val="Energy RUVY matrices"/>
+      <sheetName val="Efficiencies"/>
+      <sheetName val="Waste"/>
+      <sheetName val="Methane Combustion - EES"/>
+      <sheetName val="Tables for Paper"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="D6">
+            <v>0.1000872</v>
           </cell>
-          <cell r="E22">
-            <v>607.29999999999995</v>
+          <cell r="E6">
+            <v>11.256799999999885</v>
+          </cell>
+          <cell r="G6">
+            <v>-12065.478902397108</v>
           </cell>
         </row>
-        <row r="24">
-          <cell r="D24">
-            <v>0.10196127799999999</v>
+        <row r="29">
+          <cell r="D29">
+            <v>8.4314200000000006E-2</v>
           </cell>
-          <cell r="E24">
-            <v>31.875999999999976</v>
+          <cell r="E29">
+            <v>33.790400000000034</v>
           </cell>
-        </row>
-        <row r="27">
-          <cell r="D27">
-            <v>9.4196000000000002E-2</v>
-          </cell>
-          <cell r="E27">
-            <v>412.83199999999999</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="D28">
-            <v>3.0973762000000002E-2</v>
-          </cell>
-          <cell r="E28">
-            <v>873.60807999999997</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="D41">
-            <v>0.16731462</v>
-          </cell>
-          <cell r="E41">
-            <v>7141.5943565339712</v>
+          <cell r="G29">
+            <v>-12996.624530624733</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="27">
+          <cell r="L27">
+            <v>198.12782320839224</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
@@ -531,6 +561,8 @@
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -903,10 +935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545274DC-34DC-FF41-A18E-A55E6B091650}">
-  <dimension ref="D12:O34"/>
+  <dimension ref="D12:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:O33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,271 +987,264 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="N23" t="s">
+    <row r="22" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="P22" t="s">
         <v>6</v>
       </c>
-      <c r="O23" t="s">
+      <c r="Q22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="N24" t="s">
+    <row r="23" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="P23" t="s">
         <v>8</v>
       </c>
-      <c r="O24" t="s">
+      <c r="Q23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="N25">
-        <v>1309.8157778632656</v>
-      </c>
-      <c r="O25">
-        <v>7072531.8830895294</v>
-      </c>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>46</v>
+      </c>
+      <c r="P24">
+        <v>208.5556034</v>
+      </c>
+      <c r="Q24">
+        <v>25394.24092</v>
+      </c>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" t="s">
+        <v>32</v>
+      </c>
+      <c r="O26" t="s">
+        <v>33</v>
+      </c>
+      <c r="P26" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>41</v>
+      </c>
       <c r="F27" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="H27" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="I27" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="K27" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L27" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="M27" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N27" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="O27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="F28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" t="s">
         <v>14</v>
       </c>
-      <c r="I28" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="P27" t="s">
         <v>17</v>
       </c>
-      <c r="L28" t="s">
-        <v>15</v>
-      </c>
-      <c r="M28" t="s">
-        <v>15</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="Q27" t="s">
         <v>18</v>
       </c>
-      <c r="O28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="28" spans="4:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28">
+        <v>198.12782319999999</v>
+      </c>
+      <c r="G28">
+        <v>0.95</v>
+      </c>
+      <c r="H28">
+        <v>0.1000872</v>
+      </c>
+      <c r="I28">
+        <v>1979.5520630000001</v>
+      </c>
+      <c r="J28">
+        <v>-12065.4789</v>
+      </c>
+      <c r="K28">
+        <v>11.2568</v>
+      </c>
+      <c r="L28">
+        <v>0.94119632900000005</v>
+      </c>
+      <c r="M28">
+        <v>-6.0603522999999999E-2</v>
+      </c>
+      <c r="N28">
+        <v>-0.13762872700000001</v>
+      </c>
+      <c r="O28">
+        <v>11.119171270000001</v>
+      </c>
+      <c r="P28">
+        <v>10.46532318</v>
+      </c>
+      <c r="Q28">
+        <v>22010.978429999999</v>
+      </c>
+    </row>
+    <row r="29" spans="4:17" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29">
+        <v>10.42778017</v>
+      </c>
+      <c r="G29">
+        <v>0.05</v>
+      </c>
+      <c r="H29">
+        <v>8.4314200000000006E-2</v>
+      </c>
+      <c r="I29">
+        <v>123.67762690000001</v>
+      </c>
+      <c r="J29">
+        <v>-12996.624529999999</v>
+      </c>
+      <c r="K29">
+        <v>33.790399999999998</v>
+      </c>
+      <c r="L29">
+        <v>5.8803671000000002E-2</v>
+      </c>
+      <c r="M29">
+        <v>-2.8335509929999998</v>
+      </c>
+      <c r="N29">
+        <v>-6.4349067470000003</v>
+      </c>
+      <c r="O29">
+        <v>27.355493249999999</v>
+      </c>
+      <c r="P29">
+        <v>1.6086034279999999</v>
+      </c>
+      <c r="Q29">
+        <v>3383.2624879999998</v>
+      </c>
+    </row>
+    <row r="30" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
         <v>21</v>
       </c>
-      <c r="F29">
-        <v>881.06000000000006</v>
-      </c>
-      <c r="G29">
-        <v>0.1596882</v>
-      </c>
-      <c r="H29">
-        <v>5517.3769884061567</v>
-      </c>
-      <c r="I29">
-        <v>17.358400000000074</v>
-      </c>
-      <c r="J29">
-        <v>0.21197353787675174</v>
-      </c>
-      <c r="K29">
-        <v>-1.5512938334370325</v>
-      </c>
-      <c r="L29">
-        <v>-3.5229403607560474</v>
-      </c>
-      <c r="M29">
-        <v>13.835459639244027</v>
-      </c>
-      <c r="N29">
-        <v>2.9327513278815638</v>
-      </c>
-      <c r="O29">
-        <v>76335.446637587142</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="E30" t="s">
+      <c r="F30">
+        <v>208.5556034</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0.18440139999999999</v>
+      </c>
+      <c r="I30">
+        <v>2103.2296900000001</v>
+      </c>
+      <c r="J30">
+        <v>-12112.036179999999</v>
+      </c>
+      <c r="K30">
+        <f>($L28*K28 + $L29*K29)</f>
+        <v>12.581858400845601</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f>($L28*N28 + $L29*N29)</f>
+        <v>-0.50793179188361148</v>
+      </c>
+      <c r="O30">
+        <f>($L28*O28 + $L29*O29)</f>
+        <v>12.07392660596199</v>
+      </c>
+      <c r="P30">
+        <v>12.073926609999999</v>
+      </c>
+      <c r="Q30">
+        <v>25394.24092</v>
+      </c>
+    </row>
+    <row r="31" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" t="s">
         <v>22</v>
       </c>
-      <c r="F30">
-        <v>118.94000000000001</v>
-      </c>
-      <c r="G30">
-        <v>6.00843E-2</v>
-      </c>
-      <c r="H30">
-        <v>1979.5520626852608</v>
-      </c>
-      <c r="I30">
-        <v>1.5260000000000673</v>
-      </c>
-      <c r="J30">
-        <v>7.6052924246496442E-2</v>
-      </c>
-      <c r="K30">
-        <v>-2.5763258093856205</v>
-      </c>
-      <c r="L30">
-        <v>-5.8507563046472342</v>
-      </c>
-      <c r="M30">
-        <v>-4.3247563046471669</v>
-      </c>
-      <c r="N30">
-        <v>-0.32891036362188886</v>
-      </c>
-      <c r="O30">
-        <v>-8561.0802634753836</v>
-      </c>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="E31" t="s">
+      <c r="I31" t="s">
         <v>23</v>
       </c>
-      <c r="F31">
-        <v>111.00813284002646</v>
-      </c>
-      <c r="G31">
-        <v>5.6077400000000006E-2</v>
-      </c>
-      <c r="H31">
-        <v>1979.5520626852608</v>
-      </c>
-      <c r="I31">
-        <v>122.25799999999992</v>
-      </c>
-      <c r="J31">
-        <v>7.6052924246496442E-2</v>
-      </c>
-      <c r="K31">
-        <v>-2.5763258093856205</v>
-      </c>
-      <c r="L31">
-        <v>-5.8507563046472342</v>
-      </c>
-      <c r="M31">
-        <v>116.40724369535269</v>
-      </c>
-      <c r="N31">
-        <v>8.8531112865061079</v>
-      </c>
-      <c r="O31">
-        <v>230434.19936864119</v>
-      </c>
-    </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="E32" t="s">
+      <c r="J31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K31" t="s">
+        <v>52</v>
+      </c>
+      <c r="N31" t="s">
+        <v>52</v>
+      </c>
+      <c r="O31" t="s">
+        <v>52</v>
+      </c>
+      <c r="P31" t="s">
         <v>24</v>
       </c>
-      <c r="F32">
-        <v>198.80764502323905</v>
-      </c>
-      <c r="G32">
-        <v>1.2010999999999999E-2</v>
-      </c>
-      <c r="H32">
-        <v>16552.130965218472</v>
-      </c>
-      <c r="I32">
-        <v>410.3</v>
-      </c>
-      <c r="J32">
-        <v>0.63592061363025532</v>
-      </c>
-      <c r="K32">
-        <v>-0.45268154476892275</v>
-      </c>
-      <c r="L32">
-        <v>-1.0280258003104901</v>
-      </c>
-      <c r="M32">
-        <v>409.27197419968951</v>
-      </c>
-      <c r="N32">
-        <v>260.26448497473257</v>
-      </c>
-      <c r="O32">
-        <v>6774323.3173467768</v>
-      </c>
-    </row>
-    <row r="33" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33">
-        <v>1309.8157778632656</v>
-      </c>
-      <c r="G33">
-        <v>0.28786090000000003</v>
-      </c>
-      <c r="H33">
-        <v>26028.612078995153</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="O33">
-        <v>7072531.8830895294</v>
-      </c>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="F34" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" t="s">
-        <v>27</v>
-      </c>
-      <c r="N34" t="s">
-        <v>28</v>
-      </c>
-      <c r="O34" t="s">
+      <c r="Q31" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1233,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7457CBA-7643-2342-AA62-D18E6247C290}">
   <dimension ref="A11:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1242,78 +1267,78 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C12" s="4"/>
       <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="7">
         <v>881.06000000000006</v>
@@ -1351,11 +1376,11 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4">
         <v>118.94000000000001</v>
@@ -1395,7 +1420,7 @@
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D15" s="4">
         <v>1.249958452402667</v>
@@ -1435,7 +1460,7 @@
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D16" s="4">
         <v>9.9996676192213361</v>
@@ -1473,7 +1498,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D17" s="4">
         <v>0.38391581038081912</v>
@@ -1511,7 +1536,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4">
         <v>0.13392411990028574</v>
@@ -1549,7 +1574,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C19" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D19" s="7">
         <v>1011.7674660019052</v>
@@ -1582,10 +1607,10 @@
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1593,7 +1618,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N20" s="5" t="s">
         <v>9</v>
@@ -1712,86 +1737,86 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C28" s="4"/>
       <c r="D28" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="J29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="K29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M29" s="5" t="s">
+      <c r="N29" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D30" s="15">
         <v>88160.656904773379</v>
@@ -1831,7 +1856,7 @@
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D31" s="15">
         <v>88160.656904773379</v>
@@ -1860,16 +1885,16 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C32" s="8"/>
       <c r="D32" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -1877,7 +1902,7 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>9</v>

</xml_diff>